<commit_message>
After doing Task 1-2
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khongorzul\Documents\Python\Week2\HW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F918B7C-A497-424B-8CD3-4FDBF01928C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC06C87B-4C71-4754-BE81-4F41E6134581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="1005" windowWidth="14790" windowHeight="15495" xr2:uid="{489879BE-C2A9-4EAA-8795-529B20F48590}"/>
+    <workbookView xWindow="13950" yWindow="105" windowWidth="14790" windowHeight="15495" xr2:uid="{489879BE-C2A9-4EAA-8795-529B20F48590}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41835BD0-3C82-408D-8043-3A3A247760FB}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,10 +1229,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
       </c>
       <c r="D12" t="s">
         <v>121</v>
@@ -1261,10 +1261,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -1293,10 +1293,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>122</v>
@@ -1325,10 +1325,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
         <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
       </c>
       <c r="D15" t="s">
         <v>123</v>
@@ -1357,10 +1357,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>71</v>
       </c>
       <c r="D16" t="s">
         <v>124</v>
@@ -1389,10 +1389,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>72</v>
       </c>
       <c r="D17" t="s">
         <v>126</v>
@@ -1421,10 +1421,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
         <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
       </c>
       <c r="D18" t="s">
         <v>125</v>
@@ -1453,10 +1453,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
         <v>51</v>
-      </c>
-      <c r="C19" t="s">
-        <v>74</v>
       </c>
       <c r="D19" t="s">
         <v>127</v>
@@ -1485,10 +1485,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
         <v>116</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
       </c>
       <c r="D20" t="s">
         <v>128</v>
@@ -1517,10 +1517,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
         <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>76</v>
       </c>
       <c r="D21" t="s">
         <v>129</v>
@@ -1549,10 +1549,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s">
         <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
       </c>
       <c r="D22" t="s">
         <v>130</v>
@@ -1581,10 +1581,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
         <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>131</v>
@@ -1613,10 +1613,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
         <v>55</v>
-      </c>
-      <c r="C24" t="s">
-        <v>78</v>
       </c>
       <c r="D24" t="s">
         <v>132</v>
@@ -1645,10 +1645,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
         <v>56</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
       </c>
       <c r="D25" t="s">
         <v>159</v>
@@ -1677,10 +1677,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
         <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>80</v>
       </c>
       <c r="D26" t="s">
         <v>133</v>
@@ -1709,10 +1709,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
         <v>58</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
       </c>
       <c r="D27" t="s">
         <v>134</v>
@@ -1741,10 +1741,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
         <v>59</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
       </c>
       <c r="D28" t="s">
         <v>135</v>
@@ -1773,10 +1773,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
         <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
       </c>
       <c r="D29" t="s">
         <v>136</v>
@@ -1805,10 +1805,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
         <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
       </c>
       <c r="D30" t="s">
         <v>137</v>
@@ -1837,10 +1837,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>85</v>
       </c>
       <c r="D31" t="s">
         <v>138</v>
@@ -1869,10 +1869,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
         <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>88</v>
       </c>
       <c r="D32" t="s">
         <v>139</v>
@@ -1901,10 +1901,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
         <v>64</v>
-      </c>
-      <c r="C33" t="s">
-        <v>89</v>
       </c>
       <c r="D33" t="s">
         <v>140</v>
@@ -1933,10 +1933,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
         <v>65</v>
-      </c>
-      <c r="C34" t="s">
-        <v>90</v>
       </c>
       <c r="D34" t="s">
         <v>141</v>
@@ -1965,10 +1965,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
         <v>66</v>
-      </c>
-      <c r="C35" t="s">
-        <v>91</v>
       </c>
       <c r="D35" t="s">
         <v>142</v>
@@ -1997,10 +1997,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" t="s">
         <v>86</v>
-      </c>
-      <c r="C36" t="s">
-        <v>87</v>
       </c>
       <c r="D36" t="s">
         <v>143</v>
@@ -2029,10 +2029,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" t="s">
         <v>92</v>
-      </c>
-      <c r="C37" t="s">
-        <v>117</v>
       </c>
       <c r="D37" t="s">
         <v>144</v>
@@ -2061,10 +2061,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
         <v>93</v>
-      </c>
-      <c r="C38" t="s">
-        <v>113</v>
       </c>
       <c r="D38" t="s">
         <v>145</v>
@@ -2093,10 +2093,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" t="s">
         <v>94</v>
-      </c>
-      <c r="C39" t="s">
-        <v>118</v>
       </c>
       <c r="D39" t="s">
         <v>146</v>
@@ -2125,10 +2125,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" t="s">
         <v>84</v>
-      </c>
-      <c r="C40" t="s">
-        <v>119</v>
       </c>
       <c r="D40" t="s">
         <v>147</v>
@@ -2157,10 +2157,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" t="s">
         <v>95</v>
-      </c>
-      <c r="C41" t="s">
-        <v>120</v>
       </c>
       <c r="D41" t="s">
         <v>148</v>
@@ -2189,10 +2189,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
         <v>96</v>
-      </c>
-      <c r="C42" t="s">
-        <v>97</v>
       </c>
       <c r="D42" t="s">
         <v>149</v>
@@ -2221,10 +2221,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
         <v>115</v>
-      </c>
-      <c r="C43" t="s">
-        <v>98</v>
       </c>
       <c r="D43" t="s">
         <v>150</v>
@@ -2253,10 +2253,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" t="s">
         <v>114</v>
-      </c>
-      <c r="C44" t="s">
-        <v>99</v>
       </c>
       <c r="D44" t="s">
         <v>151</v>
@@ -2285,10 +2285,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" t="s">
         <v>112</v>
-      </c>
-      <c r="C45" t="s">
-        <v>100</v>
       </c>
       <c r="D45" t="s">
         <v>152</v>
@@ -2317,10 +2317,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" t="s">
         <v>111</v>
-      </c>
-      <c r="C46" t="s">
-        <v>101</v>
       </c>
       <c r="D46" t="s">
         <v>153</v>
@@ -2349,10 +2349,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" t="s">
         <v>110</v>
-      </c>
-      <c r="C47" t="s">
-        <v>102</v>
       </c>
       <c r="D47" t="s">
         <v>154</v>
@@ -2381,10 +2381,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" t="s">
         <v>109</v>
-      </c>
-      <c r="C48" t="s">
-        <v>103</v>
       </c>
       <c r="D48" t="s">
         <v>155</v>
@@ -2413,10 +2413,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" t="s">
         <v>105</v>
-      </c>
-      <c r="C49" t="s">
-        <v>104</v>
       </c>
       <c r="D49" t="s">
         <v>156</v>
@@ -2445,10 +2445,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" t="s">
         <v>108</v>
-      </c>
-      <c r="C50" t="s">
-        <v>106</v>
       </c>
       <c r="D50" t="s">
         <v>157</v>
@@ -2477,10 +2477,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
         <v>44</v>
-      </c>
-      <c r="C51" t="s">
-        <v>107</v>
       </c>
       <c r="D51" t="s">
         <v>158</v>

</xml_diff>